<commit_message>
Tested SIMPER OTU w/o Sex; Organized Simper code
</commit_message>
<xml_diff>
--- a/stevia.simper.all.xlsx
+++ b/stevia.simper.all.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C9CDB93E-68E9-4802-9A4A-70A7B7187B1E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663BA208-BF19-4DBA-BE2B-BB13CF0CD46E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stevia.simper.all" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,18 @@
     <sheet name="All" sheetId="3" r:id="rId3"/>
     <sheet name="Pre" sheetId="4" r:id="rId4"/>
     <sheet name="Post" sheetId="5" r:id="rId5"/>
-    <sheet name="HF" sheetId="6" r:id="rId6"/>
-    <sheet name="LF" sheetId="7" r:id="rId7"/>
-    <sheet name="SC" sheetId="8" r:id="rId8"/>
-    <sheet name="TV" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId6"/>
+    <sheet name="HF" sheetId="6" r:id="rId7"/>
+    <sheet name="LF" sheetId="7" r:id="rId8"/>
+    <sheet name="SC" sheetId="8" r:id="rId9"/>
+    <sheet name="TV" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="82">
   <si>
     <t>Comparison</t>
   </si>
@@ -279,7 +280,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1129,11 +1130,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K312"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A100" sqref="A1:XFD100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12066,12 +12067,349 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="7" max="7" width="92.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5.6212887646308302E-2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3.31065830938524E-4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3.5496068761903302E-3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>8.7062914046147299E-2</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2.8027219940559199E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.8948775551756002E-2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6.4063901472727E-4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.8594813068336797E-3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.90725072021207E-3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3.41802035655478E-3</v>
+      </c>
+      <c r="J3" s="2">
+        <v>7.7684787244468201E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.9334441345233998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4.4020216602883001E-2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.7417331272204999E-3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.3871699729866E-2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7.3416467665020399E-2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>7.7454304713007197E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5.3147724831653998E-3</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4.1604551238293101E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.1782849364061E-2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7.7753044694038305E-4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5.6235341627548603E-3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.2067010591622299E-2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8.8705547081187192E-3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.6680712901025294E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>3.6788413092938198E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.6814812086988002E-2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.53717795827587E-4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4.3051558625594897E-3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5.7467764818751599E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5.22536434700063E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1.30718963182978E-4</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2.42044498101584E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.3912004258779001E-2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.3220945158780098E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.2451230938587301E-2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="2">
+        <v>3.58069281985849E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.03760847100736E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>8.7808481282931602E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2.9561007088034899E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4.9778705993796003E-2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.1816724426084099E-3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>7.5026943003675302E-3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="2">
+        <v>6.5263961587458799E-2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>7.0328332120527998E-2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5.6296770554082602E-2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.1274615201549499E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>4.3382395636814099E-2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.0488901974788801E-3</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1.6071873263705501E-3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>7.4619928502047697E-2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>7.1004952015327694E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:K7">
+    <sortCondition descending="1" ref="C1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1048576"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15585,11 +15923,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16762,11 +17100,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD24"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16888,31 +17226,31 @@
         <v>63</v>
       </c>
       <c r="C4" s="2">
-        <v>5.5812944314101998E-2</v>
+        <v>7.0617543283187006E-2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3">
-        <v>4.4647893140438001E-6</v>
+        <v>23</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.1820965296399E-3</v>
       </c>
       <c r="F4" s="2">
-        <v>1.1571245638896801E-4</v>
+        <v>7.5026943003675302E-3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2">
-        <v>2.2905063731741199E-2</v>
+        <v>0.11416357362585</v>
       </c>
       <c r="I4" s="2">
-        <v>2.1275358928292701E-2</v>
+        <v>9.0495768738603405E-2</v>
       </c>
       <c r="J4" s="2">
-        <v>9.1802236084300798E-2</v>
+        <v>3.8618812272006198E-2</v>
       </c>
       <c r="K4" s="2">
-        <v>3.9078519986565197E-2</v>
+        <v>3.8512437627368001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -16958,44 +17296,47 @@
         <v>63</v>
       </c>
       <c r="C6" s="2">
-        <v>7.0617543283187006E-2</v>
+        <v>5.5812944314101998E-2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.1820965296399E-3</v>
+        <v>21</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4.4647893140438001E-6</v>
       </c>
       <c r="F6" s="2">
-        <v>7.5026943003675302E-3</v>
+        <v>1.1571245638896801E-4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="H6" s="2">
-        <v>0.11416357362585</v>
+        <v>2.2905063731741199E-2</v>
       </c>
       <c r="I6" s="2">
-        <v>9.0495768738603405E-2</v>
+        <v>2.1275358928292701E-2</v>
       </c>
       <c r="J6" s="2">
-        <v>3.8618812272006198E-2</v>
+        <v>9.1802236084300798E-2</v>
       </c>
       <c r="K6" s="2">
-        <v>3.8512437627368001E-2</v>
+        <v>3.9078519986565197E-2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:K6">
+    <sortCondition descending="1" ref="C1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B1:B1048576"/>
+      <selection activeCell="A4" sqref="A4:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18098,11 +18439,870 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D830C3-FF3D-4D26-B96A-D454BB549D41}">
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD69"/>
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="38.109375" customWidth="1"/>
+    <col min="7" max="7" width="88.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2">
+        <v>4.0266360684467997E-2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="3">
+        <v>7.0977311354282995E-5</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1.3560869745758901E-3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2">
+        <v>6.4456969702629693E-2</v>
+      </c>
+      <c r="K1" s="2">
+        <v>2.7301250920689999E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5.7558785434502997E-2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.3112218211929401E-4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.8356191164406802E-3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.21940685670442E-2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1.15682534014694E-2</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.104364381620143</v>
+      </c>
+      <c r="K2" s="2">
+        <v>3.0349769657808699E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.4966969809608001E-2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.35566271685926E-4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.8356191164406802E-3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3.6708805503538901E-3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3.18113014923917E-3</v>
+      </c>
+      <c r="J3" s="2">
+        <v>7.5658367581826605E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2.45131952540159E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.2586616847999003E-2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.3706140523298299E-4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2.8356191164406802E-3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8.1144190635125592E-3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>5.2721278125834803E-3</v>
+      </c>
+      <c r="J4" s="2">
+        <v>6.0303370153375502E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.8478356629546701E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.4805316655554001E-2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.46866729113481E-4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.5496068761903302E-3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3.9653470082137703E-2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5.0801681985948401E-2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8.2362464717860295E-2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3.5737568420889298E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.7366224654525898E-2</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.8969125861471401E-3</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5.8185129323184998E-3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.13291132548534301</v>
+      </c>
+      <c r="K6" s="2">
+        <v>8.8061366008365796E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4.7085638897237998E-2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6.1810810729951201E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.74616601957355E-2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2">
+        <v>7.9151089864262503E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>5.9428936240383999E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>7.0200095552167899E-3</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1.23585639435065E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.3909666369990999E-2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7.05072911042272E-3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.0455232685298098E-2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="2">
+        <v>3.3837010994044098E-2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.9212544957777002E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>6.7665559522692306E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2.6743591259859999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9.5696176194426399E-2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.8940954875338001E-4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2.67756225737733E-3</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.8969125861471401E-3</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5.8185129323184998E-3</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.15332185989663799</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.111776717751684</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.5784619149022999E-2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.3706140523298299E-4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2.8356191164406802E-3</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="2">
+        <v>8.1144190635125592E-3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5.2721278125834803E-3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>6.47654237563801E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>3.1369420650115602E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.4967718006232001E-2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5.5140369380320305E-4</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4.3051558625594897E-3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3.9653470082137703E-2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5.0801681985948401E-2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>5.8112505811250599E-5</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1.7433751743375201E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3.9805391357367999E-2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.0798362378453301E-3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7.1452993610616501E-3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3.6708805503538901E-3</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3.18113014923917E-3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>6.6422285036310397E-2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3.7559763637476602E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2.0832646564888001E-2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.0008912225346299E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.1314130367423099E-2</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3.3032612600022999E-2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2.98083230325525E-2</v>
+      </c>
+      <c r="J14" s="3">
+        <v>5.8051782189713198E-5</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.7415534656914001E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5.7425168179759997E-2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.7471881993271999E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.3871699729866E-2</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.21940685670442E-2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1.15682534014694E-2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.100423193991833</v>
+      </c>
+      <c r="K15" s="2">
+        <v>4.0870260745796E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.7679739690298997E-2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2">
+        <v>6.5600513004507302E-3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2.8734872597749001E-2</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="2">
+        <v>7.9151089864262503E-2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>5.9428936240383999E-2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>6.2830123863181798E-3</v>
+      </c>
+      <c r="K16" s="2">
+        <v>8.0234043720339293E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5.4399691116227E-2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="3">
+        <v>9.5488256257511201E-5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.6498248720047801E-3</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>8.7062914046147299E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>2.8027219940559199E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2">
+        <v>4.7213868576557003E-2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3.6622398281937698E-4</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3.5496068761903302E-3</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1.21940685670442E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1.15682534014694E-2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>8.7808481282931602E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <v>2.9561007088034899E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4.6258074942682997E-2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3.7140910089413398E-4</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3.5496068761903302E-3</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="2">
+        <v>3.6708805503538901E-3</v>
+      </c>
+      <c r="I20" s="2">
+        <v>3.18113014923917E-3</v>
+      </c>
+      <c r="J20" s="2">
+        <v>7.7684787244468201E-2</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.9334441345233998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4.2849481288587003E-2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3.766463887919E-4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>3.5496068761903302E-3</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="2">
+        <v>8.1144190635125592E-3</v>
+      </c>
+      <c r="I21" s="2">
+        <v>5.2721278125834803E-3</v>
+      </c>
+      <c r="J21" s="2">
+        <v>7.6680712901025294E-2</v>
+      </c>
+      <c r="K21" s="2">
+        <v>3.6788413092938198E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2">
+        <v>4.3335580337865998E-2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="2">
+        <v>8.1677878399501603E-4</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5.6448489293877803E-3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1.8969125861471401E-3</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5.8185129323184998E-3</v>
+      </c>
+      <c r="J22" s="2">
+        <v>7.0368073664140399E-2</v>
+      </c>
+      <c r="K22" s="2">
+        <v>6.8986188459091199E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2.4732917182339002E-2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.3398722707605201E-3</v>
+      </c>
+      <c r="F23" s="2">
+        <v>8.3340055241304407E-3</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3.9653470082137703E-2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>5.0801681985948401E-2</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1.30718963182978E-4</v>
+      </c>
+      <c r="K23" s="2">
+        <v>2.42044498101584E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2.0688947524286998E-2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.79979108505883E-3</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.0365463471357301E-2</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="2">
+        <v>3.3032612600022999E-2</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2.98083230325525E-2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2">
+        <v>4.8235023855542999E-2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4.3608415052213004E-3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2.0864949355751099E-2</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="2">
+        <v>7.9151089864262503E-2</v>
+      </c>
+      <c r="I25" s="2">
+        <v>5.9428936240383999E-2</v>
+      </c>
+      <c r="J25" s="2">
+        <v>3.8545545014287302E-3</v>
+      </c>
+      <c r="K25" s="2">
+        <v>6.3029746271439698E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2.1214086455746999E-2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="2">
+        <v>7.6857940552132499E-3</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3.2301107448261097E-2</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="2">
+        <v>3.3837010994044098E-2</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1.9212544957777002E-2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>6.2873231887820694E-2</v>
+      </c>
+      <c r="K26" s="2">
+        <v>2.75271798015095E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18154,31 +19354,31 @@
         <v>59</v>
       </c>
       <c r="C2" s="2">
-        <v>4.1306428091556997E-2</v>
+        <v>4.9090564750553997E-2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2">
-        <v>1.3311407728362401E-4</v>
+        <v>1.7201435751819001E-3</v>
       </c>
       <c r="F2" s="2">
-        <v>2.06992390176035E-3</v>
+        <v>1.00936726770108E-2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2">
-        <v>0</v>
+        <v>8.3857900411084596E-2</v>
       </c>
       <c r="I2" s="2">
-        <v>0</v>
+        <v>6.3598775104669297E-2</v>
       </c>
       <c r="J2" s="2">
-        <v>6.4456969702629693E-2</v>
+        <v>8.1224909127481492E-3</v>
       </c>
       <c r="K2" s="2">
-        <v>2.7301250920689999E-2</v>
+        <v>6.10481954377239E-3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -18224,31 +19424,31 @@
         <v>59</v>
       </c>
       <c r="C4" s="2">
-        <v>3.2509447653077998E-2</v>
+        <v>4.1306428091556997E-2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
-        <v>3.4612206766775099E-4</v>
+        <v>1.3311407728362401E-4</v>
       </c>
       <c r="F4" s="2">
-        <v>3.5496068761903302E-3</v>
+        <v>2.06992390176035E-3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2">
-        <v>9.5924514771815496E-3</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
-        <v>5.52754879778093E-3</v>
+        <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>6.0303370153375502E-2</v>
+        <v>6.4456969702629693E-2</v>
       </c>
       <c r="K4" s="2">
-        <v>1.8478356629546701E-2</v>
+        <v>2.7301250920689999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -18256,34 +19456,34 @@
         <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2">
-        <v>6.4408693797157995E-2</v>
+        <v>3.4943677324174999E-2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2">
-        <v>4.0441530242528499E-4</v>
+        <v>2.3158069098906E-3</v>
       </c>
       <c r="F5" s="2">
-        <v>3.6992105604195199E-3</v>
+        <v>1.2451230938587301E-2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2">
-        <v>0</v>
+        <v>5.1729270520396803E-2</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>1.5810362333079499E-2</v>
       </c>
       <c r="J5" s="2">
-        <v>8.3235363691491399E-2</v>
+        <v>0.104364381620143</v>
       </c>
       <c r="K5" s="2">
-        <v>9.7407065221715397E-2</v>
+        <v>3.0349769657808699E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -18294,31 +19494,31 @@
         <v>59</v>
       </c>
       <c r="C6" s="2">
-        <v>2.4176772783965E-2</v>
+        <v>3.2509447653077998E-2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2">
-        <v>4.79364928051719E-4</v>
+        <v>3.4612206766775099E-4</v>
       </c>
       <c r="F6" s="2">
-        <v>4.0292565574076896E-3</v>
+        <v>3.5496068761903302E-3</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2">
-        <v>3.7784131319383303E-2</v>
+        <v>9.5924514771815496E-3</v>
       </c>
       <c r="I6" s="2">
-        <v>2.4141008515988799E-2</v>
+        <v>5.52754879778093E-3</v>
       </c>
       <c r="J6" s="2">
-        <v>0</v>
+        <v>6.0303370153375502E-2</v>
       </c>
       <c r="K6" s="2">
-        <v>0</v>
+        <v>1.8478356629546701E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -18329,114 +19529,117 @@
         <v>59</v>
       </c>
       <c r="C7" s="2">
-        <v>4.9090564750553997E-2</v>
+        <v>2.4176772783965E-2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="E7" s="2">
-        <v>1.7201435751819001E-3</v>
+        <v>4.79364928051719E-4</v>
       </c>
       <c r="F7" s="2">
-        <v>1.00936726770108E-2</v>
+        <v>4.0292565574076896E-3</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2">
-        <v>8.3857900411084596E-2</v>
+        <v>3.7784131319383303E-2</v>
       </c>
       <c r="I7" s="2">
-        <v>6.3598775104669297E-2</v>
+        <v>2.4141008515988799E-2</v>
       </c>
       <c r="J7" s="2">
-        <v>8.1224909127481492E-3</v>
+        <v>0</v>
       </c>
       <c r="K7" s="2">
-        <v>6.10481954377239E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="2">
-        <v>3.4943677324174999E-2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2.3158069098906E-3</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.2451230938587301E-2</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5.1729270520396803E-2</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1.5810362333079499E-2</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.104364381620143</v>
-      </c>
-      <c r="K8" s="2">
-        <v>3.0349769657808699E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.4408693797157995E-2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.0441530242528499E-4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.6992105604195199E-3</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>8.3235363691491399E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>9.7407065221715397E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C11" s="2">
         <v>4.6531160431792999E-2</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E11" s="2">
         <v>7.6697647519251896E-3</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F11" s="2">
         <v>3.2301107448261097E-2</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H11" s="2">
         <v>1.3561067563498499E-2</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I11" s="2">
         <v>4.23323558278694E-2</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J11" s="2">
         <v>5.7121492851624302E-2</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K11" s="2">
         <v>6.8411814667164797E-2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:K8">
+    <sortCondition descending="1" ref="C1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18485,34 +19688,34 @@
         <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2">
-        <v>6.3835019210609995E-2</v>
+        <v>5.8250129621104998E-2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3">
-        <v>7.4126940732443999E-5</v>
+        <v>26</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.5238211861631401E-3</v>
       </c>
       <c r="F2" s="2">
-        <v>1.3560869745758901E-3</v>
+        <v>9.2212160148533902E-3</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="3">
-        <v>5.2083333333333303E-5</v>
+        <v>18</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6.0474615656430104E-3</v>
       </c>
       <c r="I2" s="2">
-        <v>1.6470196146710299E-4</v>
+        <v>1.7027980661973599E-2</v>
       </c>
       <c r="J2" s="2">
-        <v>8.1456903835032901E-2</v>
+        <v>7.9151089864262503E-2</v>
       </c>
       <c r="K2" s="2">
-        <v>5.5290712377984802E-2</v>
+        <v>5.9428936240383999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -18523,31 +19726,31 @@
         <v>59</v>
       </c>
       <c r="C3" s="2">
-        <v>5.8250129621104998E-2</v>
+        <v>3.2054439801146001E-2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2">
-        <v>1.5238211861631401E-3</v>
+        <v>8.1270246529102207E-3</v>
       </c>
       <c r="F3" s="2">
-        <v>9.2212160148533902E-3</v>
+        <v>3.3700062227400997E-2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2">
-        <v>6.0474615656430104E-3</v>
+        <v>7.1097124033316597E-2</v>
       </c>
       <c r="I3" s="2">
-        <v>1.7027980661973599E-2</v>
+        <v>3.9191884556681197E-2</v>
       </c>
       <c r="J3" s="2">
-        <v>7.9151089864262503E-2</v>
+        <v>3.3837010994044098E-2</v>
       </c>
       <c r="K3" s="2">
-        <v>5.9428936240383999E-2</v>
+        <v>1.9212544957777002E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -18585,122 +19788,125 @@
         <v>1.5422204969587801E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3.2054439801146001E-2</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6.3835019210609995E-2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.4126940732443999E-5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.3560869745758901E-3</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5.2083333333333303E-5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.6470196146710299E-4</v>
+      </c>
+      <c r="J9" s="2">
+        <v>8.1456903835032901E-2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>5.5290712377984802E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3.2853205858244E-2</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="2">
-        <v>8.1270246529102207E-3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>3.3700062227400997E-2</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="2">
-        <v>7.1097124033316597E-2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>3.9191884556681197E-2</v>
-      </c>
-      <c r="J5" s="2">
-        <v>3.3837010994044098E-2</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1.9212544957777002E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="E10" s="2">
+        <v>1.1298951918269899E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4.3382395636814099E-2</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="2">
+        <v>7.1206729508116795E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4.0619125272994501E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3.3727405519243997E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.5687903101232199E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="2">
-        <v>3.2853205858244E-2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.1298951918269899E-2</v>
-      </c>
-      <c r="F6" s="2">
-        <v>4.3382395636814099E-2</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="2">
-        <v>7.1206729508116795E-2</v>
-      </c>
-      <c r="I6" s="2">
-        <v>4.0619125272994501E-2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>3.3727405519243997E-2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1.5687903101232199E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="C11" s="4">
         <v>5.5201910547874003E-2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E11" s="4">
         <v>1.90648146819343E-2</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F11" s="4">
         <v>6.5155575451445805E-2</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H11" s="4">
         <v>2.967550198989E-2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I11" s="4">
         <v>2.7323271752167401E-2</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J11" s="4">
         <v>8.9257370652057993E-2</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K11" s="4">
         <v>5.96519714365841E-2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:K4">
+    <sortCondition descending="1" ref="C1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD19"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18752,31 +19958,31 @@
         <v>59</v>
       </c>
       <c r="C2" s="2">
-        <v>4.2246617933862002E-2</v>
+        <v>7.11877493525368E-2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2">
-        <v>6.9272204407325405E-4</v>
+        <v>2.3158069098906E-3</v>
       </c>
       <c r="F2" s="2">
-        <v>5.1294418025424303E-3</v>
+        <v>1.2451230938587301E-2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2">
-        <v>2.3983493886395799E-3</v>
+        <v>0.115047413674704</v>
       </c>
       <c r="I2" s="2">
-        <v>3.13630108047008E-3</v>
+        <v>0.114382311766388</v>
       </c>
       <c r="J2" s="2">
-        <v>6.6422285036310397E-2</v>
+        <v>7.6956290311864101E-3</v>
       </c>
       <c r="K2" s="2">
-        <v>3.7559763637476602E-2</v>
+        <v>5.8841368235440401E-3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -18787,31 +19993,31 @@
         <v>59</v>
       </c>
       <c r="C3" s="2">
-        <v>3.4761339693580001E-2</v>
+        <v>4.5177242797406002E-2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2">
-        <v>8.1120586965036795E-4</v>
+        <v>5.4105338560848596E-3</v>
       </c>
       <c r="F3" s="2">
-        <v>5.6448489293877803E-3</v>
+        <v>2.4738166848584198E-2</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2">
-        <v>5.3212368356205797E-2</v>
+        <v>4.0997007543537203E-2</v>
       </c>
       <c r="I3" s="2">
-        <v>4.20871435375186E-2</v>
-      </c>
-      <c r="J3" s="3">
-        <v>5.8112505811250599E-5</v>
+        <v>1.4149131284717901E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.100423193991833</v>
       </c>
       <c r="K3" s="2">
-        <v>1.7433751743375201E-4</v>
+        <v>4.0870260745796E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -18822,31 +20028,31 @@
         <v>59</v>
       </c>
       <c r="C4" s="2">
-        <v>3.1554866773442998E-2</v>
+        <v>4.2246617933862002E-2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2">
-        <v>1.07336005296515E-3</v>
+        <v>6.9272204407325405E-4</v>
       </c>
       <c r="F4" s="2">
-        <v>7.1452993610616501E-3</v>
+        <v>5.1294418025424303E-3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2">
-        <v>1.8407239210891001E-2</v>
+        <v>2.3983493886395799E-3</v>
       </c>
       <c r="I4" s="2">
-        <v>1.52944083353601E-2</v>
+        <v>3.13630108047008E-3</v>
       </c>
       <c r="J4" s="2">
-        <v>6.47654237563801E-2</v>
+        <v>6.6422285036310397E-2</v>
       </c>
       <c r="K4" s="2">
-        <v>3.1369420650115602E-2</v>
+        <v>3.7559763637476602E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -18857,31 +20063,31 @@
         <v>59</v>
       </c>
       <c r="C5" s="2">
-        <v>7.11877493525368E-2</v>
+        <v>3.4761339693580001E-2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2">
-        <v>2.3158069098906E-3</v>
+        <v>8.1120586965036795E-4</v>
       </c>
       <c r="F5" s="2">
-        <v>1.2451230938587301E-2</v>
+        <v>5.6448489293877803E-3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2">
-        <v>0.115047413674704</v>
+        <v>5.3212368356205797E-2</v>
       </c>
       <c r="I5" s="2">
-        <v>0.114382311766388</v>
-      </c>
-      <c r="J5" s="2">
-        <v>7.6956290311864101E-3</v>
+        <v>4.20871435375186E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5.8112505811250599E-5</v>
       </c>
       <c r="K5" s="2">
-        <v>5.8841368235440401E-3</v>
+        <v>1.7433751743375201E-4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -18892,545 +20098,211 @@
         <v>59</v>
       </c>
       <c r="C6" s="2">
-        <v>4.5177242797406002E-2</v>
+        <v>3.1554866773442998E-2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2">
-        <v>5.4105338560848596E-3</v>
+        <v>1.07336005296515E-3</v>
       </c>
       <c r="F6" s="2">
-        <v>2.4738166848584198E-2</v>
+        <v>7.1452993610616501E-3</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.8407239210891001E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.52944083353601E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>6.47654237563801E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>3.1369420650115602E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.5435796132015E-2</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.3694048102454601E-2</v>
+      </c>
+      <c r="F14" s="4">
+        <v>5.1360754270000801E-2</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2">
-        <v>4.0997007543537203E-2</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1.4149131284717901E-2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.100423193991833</v>
-      </c>
-      <c r="K6" s="2">
-        <v>4.0870260745796E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="H14" s="4">
+        <v>3.6596970129639098E-3</v>
+      </c>
+      <c r="I14" s="4">
+        <v>9.3276236612073096E-3</v>
+      </c>
+      <c r="J14" s="4">
+        <v>3.3291767159063401E-2</v>
+      </c>
+      <c r="K14" s="4">
+        <v>4.3558594343238902E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2.5681855226746E-2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.4343597030936401E-2</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5.2480690313190803E-2</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="4">
+        <v>5.7003741442615604E-3</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1.0543667727444099E-2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>4.1614690555852998E-2</v>
+      </c>
+      <c r="K15" s="4">
+        <v>3.5236241330494703E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="4">
-        <v>2.5435796132015E-2</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.3694048102454601E-2</v>
-      </c>
-      <c r="F7" s="4">
-        <v>5.1360754270000801E-2</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="C16" s="4">
+        <v>2.7864898127226999E-2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.51662664468662E-2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5.4845451918318501E-2</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="4">
+        <v>3.585016314647E-2</v>
+      </c>
+      <c r="I16" s="4">
+        <v>4.2294619007001502E-2</v>
+      </c>
+      <c r="J16" s="4">
+        <v>7.0689923462713203E-3</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1.9364349918550999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4.3576460787405999E-2</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2.8536486037148302E-2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>9.1493269665496105E-2</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="4">
+        <v>5.7290355927014501E-2</v>
+      </c>
+      <c r="I17" s="4">
+        <v>7.31946267689388E-2</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1.9692418643724299E-4</v>
+      </c>
+      <c r="K17" s="4">
+        <v>2.7178660362296199E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4.1361550414892E-2</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2.9534952177728401E-2</v>
+      </c>
+      <c r="F18" s="4">
+        <v>9.3510585069145599E-2</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="4">
-        <v>3.6596970129639098E-3</v>
-      </c>
-      <c r="I7" s="4">
-        <v>9.3276236612073096E-3</v>
-      </c>
-      <c r="J7" s="4">
-        <v>3.3291767159063401E-2</v>
-      </c>
-      <c r="K7" s="4">
-        <v>4.3558594343238902E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2.5681855226746E-2</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.4343597030936401E-2</v>
-      </c>
-      <c r="F8" s="4">
-        <v>5.2480690313190803E-2</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="4">
-        <v>5.7003741442615604E-3</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1.0543667727444099E-2</v>
-      </c>
-      <c r="J8" s="4">
-        <v>4.1614690555852998E-2</v>
-      </c>
-      <c r="K8" s="4">
-        <v>3.5236241330494703E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2.7864898127226999E-2</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.51662664468662E-2</v>
-      </c>
-      <c r="F9" s="4">
-        <v>5.4845451918318501E-2</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="4">
-        <v>3.585016314647E-2</v>
-      </c>
-      <c r="I9" s="4">
-        <v>4.2294619007001502E-2</v>
-      </c>
-      <c r="J9" s="4">
-        <v>7.0689923462713203E-3</v>
-      </c>
-      <c r="K9" s="4">
-        <v>1.9364349918550999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="4">
-        <v>4.3576460787405999E-2</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2.8536486037148302E-2</v>
-      </c>
-      <c r="F10" s="4">
-        <v>9.1493269665496105E-2</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="4">
-        <v>5.7290355927014501E-2</v>
-      </c>
-      <c r="I10" s="4">
-        <v>7.31946267689388E-2</v>
-      </c>
-      <c r="J10" s="4">
-        <v>1.9692418643724299E-4</v>
-      </c>
-      <c r="K10" s="4">
-        <v>2.7178660362296199E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="4">
-        <v>4.1361550414892E-2</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="4">
-        <v>2.9534952177728401E-2</v>
-      </c>
-      <c r="F11" s="4">
-        <v>9.3510585069145599E-2</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="H18" s="4">
         <v>6.34219431382856E-2</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I18" s="4">
         <v>7.4860585611632502E-2</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J18" s="4">
         <v>4.09051613007989E-4</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K18" s="4">
         <v>7.3371017527966995E-4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="7" max="7" width="92.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="2">
-        <v>4.9778705993796003E-2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.1816724426084099E-3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>7.5026943003675302E-3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="2">
-        <v>6.5263961587458799E-2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>7.0328332120527998E-2</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5.6296770554082602E-2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.1274615201549499E-2</v>
-      </c>
-      <c r="F3" s="2">
-        <v>4.3382395636814099E-2</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1.0488901974788801E-3</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1.6071873263705501E-3</v>
-      </c>
-      <c r="J3" s="2">
-        <v>7.4619928502047697E-2</v>
-      </c>
-      <c r="K3" s="2">
-        <v>7.1004952015327694E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="2">
-        <v>5.6212887646308302E-2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3.31065830938524E-4</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3.5496068761903302E-3</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>8.7062914046147299E-2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>2.8027219940559199E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3.6814812086988002E-2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5.53717795827587E-4</v>
-      </c>
-      <c r="F5" s="2">
-        <v>4.3051558625594897E-3</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5.7467764818751599E-2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>5.22536434700063E-2</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1.30718963182978E-4</v>
-      </c>
-      <c r="K5" s="2">
-        <v>2.42044498101584E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4.8948775551756002E-2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="2">
-        <v>6.4063901472727E-4</v>
-      </c>
-      <c r="F6" s="2">
-        <v>4.8594813068336797E-3</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1.90725072021207E-3</v>
-      </c>
-      <c r="I6" s="2">
-        <v>3.41802035655478E-3</v>
-      </c>
-      <c r="J6" s="2">
-        <v>7.7684787244468201E-2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1.9334441345233998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4.1782849364061E-2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="2">
-        <v>7.7753044694038305E-4</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5.6235341627548603E-3</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1.2067010591622299E-2</v>
-      </c>
-      <c r="I7" s="2">
-        <v>8.8705547081187192E-3</v>
-      </c>
-      <c r="J7" s="2">
-        <v>7.6680712901025294E-2</v>
-      </c>
-      <c r="K7" s="2">
-        <v>3.6788413092938198E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="2">
-        <v>3.3912004258779001E-2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2.3220945158780098E-3</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.2451230938587301E-2</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="2">
-        <v>3.58069281985849E-2</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1.03760847100736E-2</v>
-      </c>
-      <c r="J8" s="2">
-        <v>8.7808481282931602E-2</v>
-      </c>
-      <c r="K8" s="2">
-        <v>2.9561007088034899E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4.4020216602883001E-2</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2.7417331272204999E-3</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.3871699729866E-2</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="2">
-        <v>7.3416467665020399E-2</v>
-      </c>
-      <c r="I9" s="2">
-        <v>7.7454304713007197E-2</v>
-      </c>
-      <c r="J9" s="2">
-        <v>5.3147724831653998E-3</v>
-      </c>
-      <c r="K9" s="2">
-        <v>4.1604551238293101E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:K100">
-    <sortCondition ref="B1"/>
+  <sortState ref="A2:K6">
+    <sortCondition descending="1" ref="C2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>